<commit_message>
several test-cases are added
</commit_message>
<xml_diff>
--- a/L_01 Credit test cases/TestCases_Ivan_Sviridovich.xlsx
+++ b/L_01 Credit test cases/TestCases_Ivan_Sviridovich.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vince\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan.Svirydovich\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51825FE6-245B-4356-AB8B-05E5F1E81DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -51,15 +50,9 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>open the link: https://benefit.by/kredit/calculate/</t>
-  </si>
-  <si>
     <t>Ready for testing</t>
   </si>
   <si>
-    <t>A sum</t>
-  </si>
-  <si>
     <t>Repayment period</t>
   </si>
   <si>
@@ -87,12 +80,6 @@
     <t>Work experience from the last job spot</t>
   </si>
   <si>
-    <t>Age of the borrower</t>
-  </si>
-  <si>
-    <t>A month salary "BYN"</t>
-  </si>
-  <si>
     <t>purpose credit</t>
   </si>
   <si>
@@ -157,9 +144,6 @@
   </si>
   <si>
     <t>Goal</t>
-  </si>
-  <si>
-    <t>Repayment period 'days'</t>
   </si>
   <si>
     <t>valid (valid user's credit sum)</t>
@@ -177,60 +161,260 @@
     <t>Verify that after filling out all valid parameters - results are displayed</t>
   </si>
   <si>
+    <t>CM_TP_2</t>
+  </si>
+  <si>
+    <t>CM_TP_3</t>
+  </si>
+  <si>
+    <t>CM_TP_1</t>
+  </si>
+  <si>
+    <t>Req_3</t>
+  </si>
+  <si>
+    <t>Req_2</t>
+  </si>
+  <si>
+    <t>Req_1</t>
+  </si>
+  <si>
+    <t>Result is displayed</t>
+  </si>
+  <si>
+    <t>An error message is displayed</t>
+  </si>
+  <si>
+    <t>Req_4</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>A validation message of error is displayed</t>
+  </si>
+  <si>
+    <t>CM_TP_4</t>
+  </si>
+  <si>
+    <t>CM_TP_5</t>
+  </si>
+  <si>
+    <t>Req_5</t>
+  </si>
+  <si>
+    <t>CM_TP_7</t>
+  </si>
+  <si>
+    <t>CM_TP_6</t>
+  </si>
+  <si>
+    <t>Req_6</t>
+  </si>
+  <si>
+    <t>Req_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result is displayed </t>
+  </si>
+  <si>
+    <t>Average mounthly income</t>
+  </si>
+  <si>
+    <t>Borrower age</t>
+  </si>
+  <si>
+    <t>Repayment credit duration</t>
+  </si>
+  <si>
+    <t>CM_TP_8</t>
+  </si>
+  <si>
+    <t>CM_TP_9</t>
+  </si>
+  <si>
+    <t>Verify that entering invalid boundary value into "Salary note" - error is displayed</t>
+  </si>
+  <si>
+    <t>Verify that entering invalid boundary value into "Repayment credit duration" - error is displayed</t>
+  </si>
+  <si>
+    <t>Req_8</t>
+  </si>
+  <si>
+    <t>Req_9</t>
+  </si>
+  <si>
     <t>1. Out of 4 items choose "refinancing"
-2. Enter invalid values in the sum field (\ -, +, ?, a-z, A-z, -, !, *, , /)
+2. Enter 100000 and more in "Salary note"
 3. Press the button 'show'</t>
   </si>
   <si>
-    <t>1. The refinancing tab is opened
-2. All parameters are expanded
-3. Seeing all proper, entered value according to the table below
-4. Result is displayed</t>
-  </si>
-  <si>
-    <t>1. The refinancing tab is opened
-2. Seeing all proper, entered value according to the table below
-3. An error message is displayed</t>
-  </si>
-  <si>
-    <t>CM_TP_2</t>
-  </si>
-  <si>
-    <t>CM_TP_3</t>
-  </si>
-  <si>
-    <t>CM_TP_1</t>
-  </si>
-  <si>
     <t>1. Out of 4 items choose "refinancing"
-2. Enter invalid values everywhere but in the sum field (\ -, +, ?, a-z, A-z, -, !, *, , /)
+2. Enter -1 and less in "Salary note"
 3. Press the button 'show'</t>
   </si>
   <si>
-    <t>Verify that after entering invalid value into the sum field leads to error message</t>
-  </si>
-  <si>
-    <t>Verify that after entering invalid value into all fields but the sum field - result is displayed with the default parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The refinancing tab is opened
-2. Seeing all inproper, entered values
-3. Result is displayed according to automatically returned to default values </t>
-  </si>
-  <si>
-    <t>Req_3</t>
-  </si>
-  <si>
-    <t>Req_2</t>
-  </si>
-  <si>
-    <t>Req_1</t>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter -1 and less in "Repayment credit duration"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter 600 and more into "Repayment credit duration"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>Verify that entering invalid boundary value into "Repayment period" - error is displayed</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter 0 and less into "Repayment period"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>Verify that after entering invalid value into "Sum" field leads to error message</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter invalid values in "Sum" field (\ -, +, ?, a-z, A-z, -, !, *, , /)
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>Verify that entering invalid boundary value into "Sum" field - error is displayed</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter 0 and less into "Sum" field
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter 15001 and more in "Sum" field
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>CM_TP_10</t>
+  </si>
+  <si>
+    <t>Req_10</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter 1001 and more into "Repayment period"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>Verify that entering invalid boundary value into "The overall work experience" - error is displayed</t>
+  </si>
+  <si>
+    <t>CM_TP_11</t>
+  </si>
+  <si>
+    <t>Req_11</t>
+  </si>
+  <si>
+    <t>CM_TP_12</t>
+  </si>
+  <si>
+    <t>Req_12</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter -1 and less in "The overall work experience"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter 100 and more in "The overall work experience"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>CM_TP_13</t>
+  </si>
+  <si>
+    <t>Req_13</t>
+  </si>
+  <si>
+    <t>Req_14</t>
+  </si>
+  <si>
+    <t>CM_TP_14</t>
+  </si>
+  <si>
+    <t>Verify that entering invalid boundary value into "Work experience from the last job spot" - error is displayed</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter 100 and more in "Work experience from the last job spot"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter -1 and less in "Work experience from the last job spot"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>CM_TP_15</t>
+  </si>
+  <si>
+    <t>Req_15</t>
+  </si>
+  <si>
+    <t>Req_16</t>
+  </si>
+  <si>
+    <t>CM_TP_16</t>
+  </si>
+  <si>
+    <t>Verify that entering invalid boundary value into "Borrower age" - error is displayed</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter 17 and less in "Borrower age"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter 101 and more in "Borrower age"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>CM_TP_17</t>
+  </si>
+  <si>
+    <t>CM_TP_18</t>
+  </si>
+  <si>
+    <t>Req_18</t>
+  </si>
+  <si>
+    <t>Req_17</t>
+  </si>
+  <si>
+    <t>Verify that entering invalid boundary value into "Average mounthly income" - error is displayed</t>
+  </si>
+  <si>
+    <t>Verify that after entering invalid value into all fields but the "Sum" field - result is displayed with the default parameters</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter invalid values everywhere but in the "Sum" field (\ -, +, ?, a-z, A-z, -, !, *, , /)
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>1. Out of 4 items choose "refinancing"
+2. Enter -1 and less in "Average mounthly income"
+3. Press the button 'show'</t>
+  </si>
+  <si>
+    <t>All entered values are match for server data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -312,7 +496,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -328,9 +512,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -368,7 +552,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -403,23 +587,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -455,26 +622,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -647,11 +797,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,106 +848,106 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>51</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="L6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="J7" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K7" s="6">
         <v>1</v>
@@ -814,34 +964,34 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H8" s="6">
         <v>500</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K8" s="6">
         <v>240</v>
@@ -858,34 +1008,34 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B9" s="6">
         <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K9" s="6">
         <v>240</v>
@@ -902,34 +1052,34 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="H10" s="6">
         <v>500</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K10" s="6">
         <v>240</v>
@@ -946,34 +1096,34 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="H11" s="6">
         <v>500</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K11" s="6">
         <v>1</v>
@@ -990,34 +1140,34 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K12" s="6">
         <v>1</v>
@@ -1034,34 +1184,34 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H13" s="6">
         <v>500</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K13" s="6">
         <v>240</v>
@@ -1078,34 +1228,34 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B14" s="6">
         <v>1</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="J14" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K14" s="6">
         <v>1</v>
@@ -1122,34 +1272,34 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="I15" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K15" s="6">
         <v>240</v>
@@ -1166,34 +1316,34 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="H16" s="6">
         <v>500</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K16" s="6">
         <v>1</v>
@@ -1210,34 +1360,34 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B17" s="6">
         <v>5</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K17" s="6">
         <v>240</v>
@@ -1254,34 +1404,34 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="H18" s="6">
         <v>500</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K18" s="6">
         <v>240</v>
@@ -1298,34 +1448,34 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K19" s="6">
         <v>1</v>
@@ -1342,34 +1492,34 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H20" s="6">
         <v>500</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K20" s="6">
         <v>240</v>
@@ -1386,34 +1536,34 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="H21" s="6">
         <v>500</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K21" s="6">
         <v>240</v>
@@ -1430,34 +1580,34 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B22" s="6">
         <v>1</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="K22" s="6">
         <v>240</v>
@@ -1474,34 +1624,34 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="E23" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H23" s="6">
         <v>500</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K23" s="6">
         <v>1</v>
@@ -1518,34 +1668,34 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B24" s="6">
         <v>5</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="J24" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K24" s="6">
         <v>1</v>
@@ -1562,34 +1712,34 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K25" s="6">
         <v>1</v>
@@ -1606,34 +1756,34 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B26" s="6">
         <v>1</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="E26" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K26" s="6">
         <v>240</v>
@@ -1650,34 +1800,34 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H27" s="6">
         <v>500</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K27" s="6">
         <v>240</v>
@@ -1694,34 +1844,34 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K28" s="6">
         <v>240</v>
@@ -1738,34 +1888,34 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B29" s="6">
         <v>5</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="K29" s="6">
         <v>1</v>
@@ -1782,34 +1932,34 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B30" s="6">
         <v>1</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G30" s="6" t="s">
+      <c r="I30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="J30" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K30" s="6">
         <v>240</v>
@@ -1826,34 +1976,34 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K31" s="6">
         <v>240</v>
@@ -1870,34 +2020,34 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B32" s="6">
         <v>5</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J32" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="K32" s="6">
         <v>1</v>
@@ -1914,34 +2064,34 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K33" s="6">
         <v>1</v>
@@ -1958,34 +2108,34 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B34" s="6">
         <v>1</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H34" s="6" t="s">
+      <c r="J34" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K34" s="6">
         <v>1</v>
@@ -2002,34 +2152,34 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K35" s="6">
         <v>240</v>
@@ -2046,34 +2196,34 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B36" s="6">
         <v>1</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K36" s="6">
         <v>240</v>
@@ -2090,34 +2240,34 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B37" s="6">
         <v>5</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="F37" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="K37" s="6">
         <v>240</v>
@@ -2134,34 +2284,34 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K38" s="6">
         <v>1</v>
@@ -2202,82 +2352,802 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="120" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="1" t="s">
+    <row r="44" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="B53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E43" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G43" s="2" t="s">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>10</v>
+      <c r="B56" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2287,7 +3157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2299,7 +3169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>